<commit_message>
to fixed y carga masiva open
</commit_message>
<xml_diff>
--- a/public/storage/Archivos/FormatosExcel/Carga_Masiva_OE.xlsx
+++ b/public/storage/Archivos/FormatosExcel/Carga_Masiva_OE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KevinCR\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC11436E-F82F-42F8-9527-F0F2C10C0D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CF877DC-3396-4921-AEA6-662742BA5342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{71AC2B83-B0D1-4BB0-BA54-74FED2C5CE57}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>fecha</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>com_part</t>
+  </si>
+  <si>
+    <t>no_control</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A784B74C-288C-4781-8FDB-9DE2BD6605E2}">
-  <dimension ref="A1:G466"/>
+  <dimension ref="A1:H466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,11 +421,12 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,2037 +446,2505 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="E3" s="2"/>
       <c r="F3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="E4" s="2"/>
       <c r="F4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="E5" s="2"/>
       <c r="F5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="E6" s="2"/>
       <c r="F6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="E7" s="2"/>
       <c r="F7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="E8" s="2"/>
       <c r="F8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="E9" s="2"/>
       <c r="F9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="E12" s="2"/>
       <c r="F12"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="E13" s="2"/>
       <c r="F13"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="E14" s="2"/>
       <c r="F14"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="E15" s="2"/>
       <c r="F15"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="E16" s="2"/>
       <c r="F16"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="E17" s="2"/>
       <c r="F17"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="E18" s="2"/>
       <c r="F18"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="E19" s="2"/>
       <c r="F19"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="E20" s="2"/>
       <c r="F20"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="E21" s="2"/>
       <c r="F21"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="E22" s="2"/>
       <c r="F22"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="E23" s="2"/>
       <c r="F23"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="E24" s="2"/>
       <c r="F24"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="E25" s="2"/>
       <c r="F25"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="E26" s="2"/>
       <c r="F26"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="E27" s="2"/>
       <c r="F27"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="E28" s="2"/>
       <c r="F28"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="E29" s="2"/>
       <c r="F29"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="E30" s="2"/>
       <c r="F30"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="E31" s="2"/>
       <c r="F31"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="E32" s="2"/>
       <c r="F32"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="E33" s="2"/>
       <c r="F33"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="E34" s="2"/>
       <c r="F34"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="E35" s="2"/>
       <c r="F35"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="E36" s="2"/>
       <c r="F36"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="E37" s="2"/>
       <c r="F37"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="E38" s="2"/>
       <c r="F38"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="E39" s="2"/>
       <c r="F39"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="E40" s="2"/>
       <c r="F40"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="E41" s="2"/>
       <c r="F41"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="E42" s="2"/>
       <c r="F42"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="E43" s="2"/>
       <c r="F43"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="E44" s="2"/>
       <c r="F44"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="E45" s="2"/>
       <c r="F45"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="E46" s="2"/>
       <c r="F46"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="E47" s="2"/>
       <c r="F47"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="E48" s="2"/>
       <c r="F48"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="E49" s="2"/>
       <c r="F49"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="E50" s="2"/>
       <c r="F50"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="E51" s="2"/>
       <c r="F51"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="E52" s="2"/>
       <c r="F52"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="E53" s="2"/>
       <c r="F53"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="E54" s="2"/>
       <c r="F54"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="E55" s="2"/>
       <c r="F55"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="E56" s="2"/>
       <c r="F56"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="E57" s="2"/>
       <c r="F57"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="E58" s="2"/>
       <c r="F58"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="E59" s="2"/>
       <c r="F59"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="E60" s="2"/>
       <c r="F60"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="E61" s="2"/>
       <c r="F61"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="E62" s="2"/>
       <c r="F62"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="E63" s="2"/>
       <c r="F63"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="E64" s="2"/>
       <c r="F64"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="E65" s="2"/>
       <c r="F65"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="E66" s="2"/>
       <c r="F66"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="E67" s="2"/>
       <c r="F67"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="E68" s="2"/>
       <c r="F68"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="E69" s="2"/>
       <c r="F69"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="E70" s="2"/>
       <c r="F70"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="E71" s="2"/>
       <c r="F71"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="E72" s="2"/>
       <c r="F72"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="E73" s="2"/>
       <c r="F73"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="E74" s="2"/>
       <c r="F74"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="E75" s="2"/>
       <c r="F75"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="E76" s="2"/>
       <c r="F76"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="E77" s="2"/>
       <c r="F77"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="E78" s="2"/>
       <c r="F78"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="E79" s="2"/>
       <c r="F79"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="E80" s="2"/>
       <c r="F80"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="E81" s="2"/>
       <c r="F81"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="E82" s="2"/>
       <c r="F82"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="E83" s="2"/>
       <c r="F83"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="E84" s="2"/>
       <c r="F84"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="E85" s="2"/>
       <c r="F85"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="E86" s="2"/>
       <c r="F86"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="E87" s="2"/>
       <c r="F87"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="E88" s="2"/>
       <c r="F88"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="E89" s="2"/>
       <c r="F89"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="E90" s="2"/>
       <c r="F90"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="E91" s="2"/>
       <c r="F91"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="E92" s="2"/>
       <c r="F92"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="E93" s="2"/>
       <c r="F93"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="E94" s="2"/>
       <c r="F94"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="E95" s="2"/>
       <c r="F95"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="E96" s="2"/>
       <c r="F96"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="E97" s="2"/>
       <c r="F97"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G97"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="E98" s="2"/>
       <c r="F98"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G98"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="E99" s="2"/>
       <c r="F99"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G99"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="E100" s="2"/>
       <c r="F100"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G100"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="E101" s="2"/>
       <c r="F101"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G101"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="E102" s="2"/>
       <c r="F102"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G102"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="E103" s="2"/>
       <c r="F103"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G103"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="E104" s="2"/>
       <c r="F104"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G104"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="E105" s="2"/>
       <c r="F105"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G105"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="E106" s="2"/>
       <c r="F106"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G106"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="E107" s="2"/>
       <c r="F107"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G107"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="E108" s="2"/>
       <c r="F108"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G108"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="E109" s="2"/>
       <c r="F109"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G109"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="E110" s="2"/>
       <c r="F110"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G110"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="E111" s="2"/>
       <c r="F111"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G111"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="E112" s="2"/>
       <c r="F112"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G112"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="E113" s="2"/>
       <c r="F113"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G113"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="E114" s="2"/>
       <c r="F114"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G114"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="E115" s="2"/>
       <c r="F115"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G115"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="E116" s="2"/>
       <c r="F116"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G116"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="E117" s="2"/>
       <c r="F117"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G117"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="E118" s="2"/>
       <c r="F118"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G118"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="E119" s="2"/>
       <c r="F119"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G119"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="E120" s="2"/>
       <c r="F120"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G120"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="E121" s="2"/>
       <c r="F121"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G121"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="E122" s="2"/>
       <c r="F122"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G122"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="E123" s="2"/>
       <c r="F123"/>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G123"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="E124" s="2"/>
       <c r="F124"/>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G124"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="E125" s="2"/>
       <c r="F125"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G125"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="E126" s="2"/>
       <c r="F126"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G126"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="E127" s="2"/>
       <c r="F127"/>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G127"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="E128" s="2"/>
       <c r="F128"/>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G128"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="E129" s="2"/>
       <c r="F129"/>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G129"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="E130" s="2"/>
       <c r="F130"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G130"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="E131" s="2"/>
       <c r="F131"/>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G131"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="E132" s="2"/>
       <c r="F132"/>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G132"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="E133" s="2"/>
       <c r="F133"/>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G133"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="E134" s="2"/>
       <c r="F134"/>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G134"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="E135" s="2"/>
       <c r="F135"/>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G135"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="E136" s="2"/>
       <c r="F136"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G136"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="E137" s="2"/>
       <c r="F137"/>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G137"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="E138" s="2"/>
       <c r="F138"/>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G138"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="E139" s="2"/>
       <c r="F139"/>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G139"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="E140" s="2"/>
       <c r="F140"/>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G140"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="E141" s="2"/>
       <c r="F141"/>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G141"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="E142" s="2"/>
       <c r="F142"/>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G142"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="E143" s="2"/>
       <c r="F143"/>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G143"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="E144" s="2"/>
       <c r="F144"/>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G144"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="E145" s="2"/>
       <c r="F145"/>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G145"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="E146" s="2"/>
       <c r="F146"/>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G146"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="E147" s="2"/>
       <c r="F147"/>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G147"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="E148" s="2"/>
       <c r="F148"/>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G148"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="E149" s="2"/>
       <c r="F149"/>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G149"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="E150" s="2"/>
       <c r="F150"/>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G150"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="E151" s="2"/>
       <c r="F151"/>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G151"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="E152" s="2"/>
       <c r="F152"/>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G152"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="E153" s="2"/>
       <c r="F153"/>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G153"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="E154" s="2"/>
       <c r="F154"/>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G154"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="E155" s="2"/>
       <c r="F155"/>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G155"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="E156" s="2"/>
       <c r="F156"/>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G156"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="E157" s="2"/>
       <c r="F157"/>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G157"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="E158" s="2"/>
       <c r="F158"/>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G158"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="E159" s="2"/>
       <c r="F159"/>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G159"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="E160" s="2"/>
       <c r="F160"/>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G160"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="E161" s="2"/>
       <c r="F161"/>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G161"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="E162" s="2"/>
       <c r="F162"/>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G162"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="E163" s="2"/>
       <c r="F163"/>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G163"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="E164" s="2"/>
       <c r="F164"/>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G164"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="E165" s="2"/>
       <c r="F165"/>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G165"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="E166" s="2"/>
       <c r="F166"/>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G166"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="E167" s="2"/>
       <c r="F167"/>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G167"/>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="E168" s="2"/>
       <c r="F168"/>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G168"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="E169" s="2"/>
       <c r="F169"/>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G169"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="E170" s="2"/>
       <c r="F170"/>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G170"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="F171"/>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G171"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="F172"/>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G172"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="F173"/>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G173"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="F174"/>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G174"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="F175"/>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G175"/>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="F176"/>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G176"/>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="F177"/>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G177"/>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="F178"/>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G178"/>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="F179"/>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G179"/>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="F180"/>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G180"/>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="F181"/>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G181"/>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="F182"/>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G182"/>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="F183"/>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G183"/>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="F184"/>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G184"/>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="F185"/>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G185"/>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="F186"/>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G186"/>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="F187"/>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G187"/>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="F188"/>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G188"/>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="F189"/>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G189"/>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="F190"/>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G190"/>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="F191"/>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G191"/>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="F192"/>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G192"/>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="F193"/>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G193"/>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="F194"/>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G194"/>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="F195"/>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G195"/>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="F196"/>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G196"/>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="F197"/>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G197"/>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="F198"/>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G198"/>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="F199"/>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G199"/>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="F200"/>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G200"/>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="F201"/>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G201"/>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="F202"/>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G202"/>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="F203"/>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G203"/>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="F204"/>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G204"/>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="F205"/>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G205"/>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="F206"/>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G206"/>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="F207"/>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G207"/>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="F208"/>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G208"/>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="F209"/>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G209"/>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="F210"/>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G210"/>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="F211"/>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G211"/>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="F212"/>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G212"/>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="F213"/>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G213"/>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="F214"/>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G214"/>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="F215"/>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G215"/>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="F216"/>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G216"/>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="F217"/>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G217"/>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="F218"/>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G218"/>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="F219"/>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G219"/>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="F220"/>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G220"/>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="F221"/>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G221"/>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="F222"/>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G222"/>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="F223"/>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G223"/>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="F224"/>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G224"/>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
       <c r="F225"/>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G225"/>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="F226"/>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G226"/>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="F227"/>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G227"/>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="1"/>
       <c r="F228"/>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G228"/>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
       <c r="F229"/>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G229"/>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="F230"/>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G230"/>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
       <c r="F231"/>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G231"/>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
       <c r="F232"/>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G232"/>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="F233"/>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G233"/>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
       <c r="F234"/>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G234"/>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
       <c r="F235"/>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G235"/>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
       <c r="F236"/>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G236"/>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
       <c r="F237"/>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G237"/>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="1"/>
       <c r="F238"/>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G238"/>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
       <c r="F239"/>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G239"/>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
       <c r="F240"/>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G240"/>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
       <c r="F241"/>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G241"/>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1"/>
       <c r="F242"/>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G242"/>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1"/>
       <c r="F243"/>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G243"/>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="1"/>
       <c r="F244"/>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G244"/>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="1"/>
       <c r="F245"/>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G245"/>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="1"/>
       <c r="F246"/>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G246"/>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="1"/>
       <c r="F247"/>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G247"/>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="1"/>
       <c r="F248"/>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G248"/>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1"/>
       <c r="F249"/>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G249"/>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="F250"/>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G250"/>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="1"/>
       <c r="F251"/>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G251"/>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="1"/>
       <c r="F252"/>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G252"/>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="1"/>
       <c r="F253"/>
-    </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G253"/>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="1"/>
       <c r="F254"/>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G254"/>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="1"/>
       <c r="F255"/>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G255"/>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="1"/>
       <c r="F256"/>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G256"/>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="1"/>
       <c r="F257"/>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G257"/>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="1"/>
       <c r="F258"/>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G258"/>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="1"/>
       <c r="F259"/>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G259"/>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="1"/>
       <c r="F260"/>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G260"/>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="1"/>
       <c r="F261"/>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G261"/>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="1"/>
       <c r="F262"/>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G262"/>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="1"/>
       <c r="F263"/>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G263"/>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="1"/>
       <c r="F264"/>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G264"/>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" s="1"/>
       <c r="F265"/>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G265"/>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="1"/>
       <c r="F266"/>
-    </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G266"/>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" s="1"/>
       <c r="F267"/>
-    </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G267"/>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="1"/>
       <c r="F268"/>
-    </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G268"/>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" s="1"/>
       <c r="F269"/>
-    </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G269"/>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" s="1"/>
       <c r="F270"/>
-    </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G270"/>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" s="1"/>
       <c r="F271"/>
-    </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G271"/>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="1"/>
       <c r="F272"/>
-    </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G272"/>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="1"/>
       <c r="F273"/>
-    </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G273"/>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="1"/>
       <c r="F274"/>
-    </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G274"/>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="1"/>
       <c r="F275"/>
-    </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G275"/>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="1"/>
       <c r="F276"/>
-    </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G276"/>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="1"/>
       <c r="F277"/>
-    </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G277"/>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" s="1"/>
       <c r="F278"/>
-    </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G278"/>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="1"/>
       <c r="F279"/>
-    </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G279"/>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="1"/>
       <c r="F280"/>
-    </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G280"/>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="1"/>
       <c r="F281"/>
-    </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G281"/>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" s="1"/>
       <c r="F282"/>
-    </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G282"/>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="1"/>
       <c r="F283"/>
-    </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G283"/>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A284" s="1"/>
       <c r="F284"/>
-    </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G284"/>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A285" s="1"/>
       <c r="F285"/>
-    </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G285"/>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A286" s="1"/>
       <c r="F286"/>
-    </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G286"/>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A287" s="1"/>
       <c r="F287"/>
-    </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G287"/>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" s="1"/>
       <c r="F288"/>
-    </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G288"/>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289" s="1"/>
       <c r="F289"/>
-    </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G289"/>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A290" s="1"/>
       <c r="F290"/>
-    </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G290"/>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" s="1"/>
       <c r="F291"/>
-    </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G291"/>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="1"/>
       <c r="F292"/>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G292"/>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" s="1"/>
       <c r="F293"/>
-    </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G293"/>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" s="1"/>
       <c r="F294"/>
-    </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G294"/>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295" s="1"/>
       <c r="F295"/>
-    </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G295"/>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A296" s="1"/>
       <c r="F296"/>
-    </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G296"/>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="1"/>
       <c r="F297"/>
-    </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G297"/>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298" s="1"/>
       <c r="F298"/>
-    </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G298"/>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A299" s="1"/>
       <c r="F299"/>
-    </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G299"/>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300" s="1"/>
       <c r="F300"/>
-    </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G300"/>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A301" s="1"/>
       <c r="F301"/>
-    </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G301"/>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302" s="1"/>
       <c r="F302"/>
-    </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G302"/>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A303" s="1"/>
       <c r="F303"/>
-    </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G303"/>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A304" s="1"/>
       <c r="F304"/>
-    </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G304"/>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A305" s="1"/>
       <c r="F305"/>
-    </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G305"/>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A306" s="1"/>
       <c r="F306"/>
-    </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G306"/>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A307" s="1"/>
       <c r="F307"/>
-    </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G307"/>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A308" s="1"/>
       <c r="F308"/>
-    </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G308"/>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A309" s="1"/>
       <c r="F309"/>
-    </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G309"/>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A310" s="1"/>
       <c r="F310"/>
-    </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G310"/>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A311" s="1"/>
       <c r="F311"/>
-    </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G311"/>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A312" s="1"/>
       <c r="F312"/>
-    </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G312"/>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A313" s="1"/>
       <c r="F313"/>
-    </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G313"/>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A314" s="1"/>
       <c r="F314"/>
-    </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G314"/>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A315" s="1"/>
       <c r="F315"/>
-    </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G315"/>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A316" s="1"/>
       <c r="F316"/>
-    </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G316"/>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A317" s="1"/>
       <c r="F317"/>
-    </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G317"/>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A318" s="1"/>
       <c r="F318"/>
-    </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G318"/>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A319" s="1"/>
       <c r="F319"/>
-    </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G319"/>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A320" s="1"/>
       <c r="F320"/>
-    </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G320"/>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A321" s="1"/>
       <c r="F321"/>
-    </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G321"/>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A322" s="1"/>
       <c r="F322"/>
-    </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G322"/>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A323" s="1"/>
       <c r="F323"/>
-    </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G323"/>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A324" s="1"/>
       <c r="F324"/>
-    </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G324"/>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A325" s="1"/>
       <c r="F325"/>
-    </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G325"/>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A326" s="1"/>
       <c r="F326"/>
-    </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G326"/>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A327" s="1"/>
       <c r="F327"/>
-    </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G327"/>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A328" s="1"/>
       <c r="F328"/>
-    </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G328"/>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A329" s="1"/>
       <c r="F329"/>
-    </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G329"/>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A330" s="1"/>
       <c r="F330"/>
-    </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G330"/>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A331" s="1"/>
       <c r="F331"/>
-    </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G331"/>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A332" s="1"/>
       <c r="F332"/>
-    </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G332"/>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A333" s="1"/>
       <c r="F333"/>
-    </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G333"/>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A334" s="1"/>
       <c r="F334"/>
-    </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G334"/>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A335" s="1"/>
       <c r="F335"/>
-    </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G335"/>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A336" s="1"/>
       <c r="F336"/>
-    </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G336"/>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A337" s="1"/>
       <c r="F337"/>
-    </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G337"/>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A338" s="1"/>
       <c r="F338"/>
-    </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G338"/>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A339" s="1"/>
       <c r="F339"/>
-    </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G339"/>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A340" s="1"/>
       <c r="F340"/>
-    </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G340"/>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A341" s="1"/>
       <c r="F341"/>
-    </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G341"/>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A342" s="1"/>
       <c r="F342"/>
-    </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G342"/>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A343" s="1"/>
       <c r="F343"/>
-    </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G343"/>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A344" s="1"/>
       <c r="F344"/>
-    </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G344"/>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A345" s="1"/>
       <c r="F345"/>
-    </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G345"/>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A346" s="1"/>
       <c r="F346"/>
-    </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G346"/>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A347" s="1"/>
       <c r="F347"/>
-    </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G347"/>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A348" s="1"/>
       <c r="F348"/>
-    </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G348"/>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" s="1"/>
       <c r="F349"/>
-    </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G349"/>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A350" s="1"/>
       <c r="F350"/>
-    </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G350"/>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A351" s="1"/>
       <c r="F351"/>
-    </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G351"/>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A352" s="1"/>
       <c r="F352"/>
-    </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G352"/>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A353" s="1"/>
       <c r="F353"/>
-    </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G353"/>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A354" s="1"/>
       <c r="F354"/>
-    </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G354"/>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A355" s="1"/>
       <c r="F355"/>
-    </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G355"/>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A356" s="1"/>
       <c r="F356"/>
-    </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G356"/>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A357" s="1"/>
       <c r="F357"/>
-    </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G357"/>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A358" s="1"/>
       <c r="F358"/>
-    </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G358"/>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A359" s="1"/>
       <c r="F359"/>
-    </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G359"/>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A360" s="1"/>
       <c r="F360"/>
-    </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G360"/>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A361" s="1"/>
       <c r="F361"/>
-    </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G361"/>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A362" s="1"/>
       <c r="F362"/>
-    </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G362"/>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A363" s="1"/>
       <c r="F363"/>
-    </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G363"/>
+    </row>
+    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A364" s="1"/>
       <c r="F364"/>
-    </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G364"/>
+    </row>
+    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A365" s="1"/>
       <c r="F365"/>
-    </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G365"/>
+    </row>
+    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A366" s="1"/>
       <c r="F366"/>
-    </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G366"/>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A367" s="1"/>
       <c r="F367"/>
-    </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G367"/>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A368" s="1"/>
       <c r="F368"/>
-    </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G368"/>
+    </row>
+    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A369" s="1"/>
       <c r="F369"/>
-    </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G369"/>
+    </row>
+    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A370" s="1"/>
       <c r="F370"/>
-    </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G370"/>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A371" s="1"/>
       <c r="F371"/>
-    </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G371"/>
+    </row>
+    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372" s="1"/>
       <c r="F372"/>
-    </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G372"/>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A373" s="1"/>
       <c r="F373"/>
-    </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G373"/>
+    </row>
+    <row r="374" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A374" s="1"/>
       <c r="F374"/>
-    </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G374"/>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A375" s="1"/>
       <c r="F375"/>
-    </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G375"/>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A376" s="1"/>
       <c r="F376"/>
-    </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G376"/>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A377" s="1"/>
       <c r="F377"/>
-    </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G377"/>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A378" s="1"/>
       <c r="F378"/>
-    </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G378"/>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A379" s="1"/>
       <c r="F379"/>
-    </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G379"/>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A380" s="1"/>
       <c r="F380"/>
-    </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G380"/>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A381" s="1"/>
       <c r="F381"/>
-    </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G381"/>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A382" s="1"/>
       <c r="F382"/>
-    </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G382"/>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A383" s="1"/>
       <c r="F383"/>
-    </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G383"/>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A384" s="1"/>
       <c r="F384"/>
-    </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G384"/>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A385" s="1"/>
       <c r="F385"/>
-    </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G385"/>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A386" s="1"/>
       <c r="F386"/>
-    </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G386"/>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A387" s="1"/>
       <c r="F387"/>
-    </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G387"/>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A388" s="1"/>
       <c r="F388"/>
-    </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G388"/>
+    </row>
+    <row r="389" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A389" s="1"/>
       <c r="F389"/>
-    </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G389"/>
+    </row>
+    <row r="390" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A390" s="1"/>
       <c r="F390"/>
-    </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G390"/>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A391" s="1"/>
       <c r="F391"/>
-    </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G391"/>
+    </row>
+    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A392" s="1"/>
       <c r="F392"/>
-    </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G392"/>
+    </row>
+    <row r="393" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A393" s="1"/>
       <c r="F393"/>
-    </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G393"/>
+    </row>
+    <row r="394" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A394" s="1"/>
       <c r="F394"/>
-    </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G394"/>
+    </row>
+    <row r="395" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A395" s="1"/>
       <c r="F395"/>
-    </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G395"/>
+    </row>
+    <row r="396" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A396" s="1"/>
       <c r="F396"/>
-    </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G396"/>
+    </row>
+    <row r="397" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A397" s="1"/>
       <c r="F397"/>
-    </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G397"/>
+    </row>
+    <row r="398" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A398" s="1"/>
       <c r="F398"/>
-    </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G398"/>
+    </row>
+    <row r="399" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A399" s="1"/>
       <c r="F399"/>
-    </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G399"/>
+    </row>
+    <row r="400" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A400" s="1"/>
       <c r="F400"/>
-    </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G400"/>
+    </row>
+    <row r="401" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A401" s="1"/>
       <c r="F401"/>
-    </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G401"/>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A402" s="1"/>
       <c r="F402"/>
-    </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G402"/>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A403" s="1"/>
       <c r="F403"/>
-    </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G403"/>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A404" s="1"/>
       <c r="F404"/>
-    </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G404"/>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A405" s="1"/>
       <c r="F405"/>
-    </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G405"/>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A406" s="1"/>
       <c r="F406"/>
-    </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G406"/>
+    </row>
+    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A407" s="1"/>
       <c r="F407"/>
-    </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G407"/>
+    </row>
+    <row r="408" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A408" s="1"/>
       <c r="F408"/>
-    </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G408"/>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A409" s="1"/>
       <c r="F409"/>
-    </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G409"/>
+    </row>
+    <row r="410" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A410" s="1"/>
       <c r="F410"/>
-    </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G410"/>
+    </row>
+    <row r="411" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A411" s="1"/>
       <c r="F411"/>
-    </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G411"/>
+    </row>
+    <row r="412" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A412" s="1"/>
       <c r="F412"/>
-    </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G412"/>
+    </row>
+    <row r="413" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A413" s="1"/>
       <c r="F413"/>
-    </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G413"/>
+    </row>
+    <row r="414" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A414" s="1"/>
       <c r="F414"/>
-    </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G414"/>
+    </row>
+    <row r="415" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A415" s="1"/>
       <c r="F415"/>
-    </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G415"/>
+    </row>
+    <row r="416" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A416" s="1"/>
       <c r="F416"/>
-    </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G416"/>
+    </row>
+    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A417" s="1"/>
       <c r="F417"/>
-    </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G417"/>
+    </row>
+    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A418" s="1"/>
       <c r="F418"/>
-    </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G418"/>
+    </row>
+    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A419" s="1"/>
       <c r="F419"/>
-    </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G419"/>
+    </row>
+    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A420" s="1"/>
       <c r="F420"/>
-    </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G420"/>
+    </row>
+    <row r="421" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A421" s="1"/>
       <c r="F421"/>
-    </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G421"/>
+    </row>
+    <row r="422" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A422" s="1"/>
       <c r="F422"/>
-    </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G422"/>
+    </row>
+    <row r="423" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A423" s="1"/>
       <c r="F423"/>
-    </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G423"/>
+    </row>
+    <row r="424" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A424" s="1"/>
       <c r="F424"/>
-    </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G424"/>
+    </row>
+    <row r="425" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A425" s="1"/>
       <c r="F425"/>
-    </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G425"/>
+    </row>
+    <row r="426" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A426" s="1"/>
       <c r="F426"/>
-    </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G426"/>
+    </row>
+    <row r="427" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A427" s="1"/>
       <c r="F427"/>
-    </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G427"/>
+    </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A428" s="1"/>
       <c r="F428"/>
-    </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G428"/>
+    </row>
+    <row r="429" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A429" s="1"/>
       <c r="F429"/>
-    </row>
-    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G429"/>
+    </row>
+    <row r="430" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A430" s="1"/>
       <c r="F430"/>
-    </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G430"/>
+    </row>
+    <row r="431" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A431" s="1"/>
       <c r="F431"/>
-    </row>
-    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G431"/>
+    </row>
+    <row r="432" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A432" s="1"/>
       <c r="F432"/>
-    </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G432"/>
+    </row>
+    <row r="433" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A433" s="1"/>
       <c r="F433"/>
-    </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G433"/>
+    </row>
+    <row r="434" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A434" s="1"/>
       <c r="F434"/>
-    </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G434"/>
+    </row>
+    <row r="435" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A435" s="1"/>
       <c r="F435"/>
-    </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G435"/>
+    </row>
+    <row r="436" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A436" s="1"/>
       <c r="F436"/>
-    </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G436"/>
+    </row>
+    <row r="437" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A437" s="1"/>
       <c r="F437"/>
-    </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G437"/>
+    </row>
+    <row r="438" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A438" s="1"/>
       <c r="F438"/>
-    </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G438"/>
+    </row>
+    <row r="439" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A439" s="1"/>
       <c r="F439"/>
-    </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G439"/>
+    </row>
+    <row r="440" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A440" s="1"/>
       <c r="F440"/>
-    </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G440"/>
+    </row>
+    <row r="441" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A441" s="1"/>
       <c r="F441"/>
-    </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G441"/>
+    </row>
+    <row r="442" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A442" s="1"/>
       <c r="F442"/>
-    </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G442"/>
+    </row>
+    <row r="443" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A443" s="1"/>
       <c r="F443"/>
-    </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G443"/>
+    </row>
+    <row r="444" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A444" s="1"/>
       <c r="F444"/>
-    </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G444"/>
+    </row>
+    <row r="445" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A445" s="1"/>
       <c r="F445"/>
-    </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G445"/>
+    </row>
+    <row r="446" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A446" s="1"/>
       <c r="F446"/>
-    </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G446"/>
+    </row>
+    <row r="447" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A447" s="1"/>
       <c r="F447"/>
-    </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G447"/>
+    </row>
+    <row r="448" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A448" s="1"/>
       <c r="F448"/>
-    </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G448"/>
+    </row>
+    <row r="449" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A449" s="1"/>
       <c r="F449"/>
-    </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G449"/>
+    </row>
+    <row r="450" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A450" s="1"/>
       <c r="F450"/>
-    </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G450"/>
+    </row>
+    <row r="451" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A451" s="1"/>
       <c r="F451"/>
-    </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G451"/>
+    </row>
+    <row r="452" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A452" s="1"/>
       <c r="F452"/>
-    </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G452"/>
+    </row>
+    <row r="453" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A453" s="1"/>
       <c r="F453"/>
-    </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G453"/>
+    </row>
+    <row r="454" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A454" s="1"/>
       <c r="F454"/>
-    </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G454"/>
+    </row>
+    <row r="455" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A455" s="1"/>
       <c r="F455"/>
-    </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G455"/>
+    </row>
+    <row r="456" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A456" s="1"/>
       <c r="F456"/>
-    </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G456"/>
+    </row>
+    <row r="457" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A457" s="1"/>
       <c r="F457"/>
-    </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G457"/>
+    </row>
+    <row r="458" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A458" s="1"/>
       <c r="F458"/>
-    </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G458"/>
+    </row>
+    <row r="459" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A459" s="1"/>
       <c r="F459"/>
-    </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G459"/>
+    </row>
+    <row r="460" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A460" s="1"/>
       <c r="F460"/>
-    </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G460"/>
+    </row>
+    <row r="461" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A461" s="1"/>
       <c r="F461"/>
-    </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G461"/>
+    </row>
+    <row r="462" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A462" s="1"/>
       <c r="F462"/>
-    </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G462"/>
+    </row>
+    <row r="463" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A463" s="1"/>
       <c r="F463"/>
-    </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G463"/>
+    </row>
+    <row r="464" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A464" s="1"/>
       <c r="F464"/>
-    </row>
-    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G464"/>
+    </row>
+    <row r="465" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A465" s="1"/>
       <c r="F465"/>
-    </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G465"/>
+    </row>
+    <row r="466" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A466" s="1"/>
       <c r="F466"/>
+      <c r="G466"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>